<commit_message>
atualiza planilhas 17 robôs
</commit_message>
<xml_diff>
--- a/sum.xlsx
+++ b/sum.xlsx
@@ -9,14 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="titulo_resumido" sheetId="2" r:id="rId2"/>
+    <sheet name="titulo_resumido" sheetId="5" r:id="rId2"/>
     <sheet name="TOTAIS" sheetId="4" r:id="rId3"/>
-    <sheet name="diff_robos" sheetId="5" r:id="rId4"/>
+    <sheet name="diff" sheetId="2" r:id="rId4"/>
     <sheet name="exceto transf-patrim-SIAD" sheetId="3" r:id="rId5"/>
+    <sheet name="ocorrências" sheetId="6" r:id="rId6"/>
+    <sheet name="Planilha4" sheetId="8" r:id="rId7"/>
+    <sheet name="horas" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="37">
   <si>
     <t>Humano: número de ocorrências</t>
   </si>
@@ -127,6 +130,18 @@
   </si>
   <si>
     <t>semanas produtivas poupadas</t>
+  </si>
+  <si>
+    <t>Humano: nº ocorrências</t>
+  </si>
+  <si>
+    <t>Humano: nº horas</t>
+  </si>
+  <si>
+    <t>Robô: nº ocorrências</t>
+  </si>
+  <si>
+    <t>Robô: ocorrências a mais</t>
   </si>
 </sst>
 </file>
@@ -135,7 +150,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -226,7 +241,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +526,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,280 +1011,487 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="G1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="8">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>30</v>
+      </c>
+      <c r="E2" s="7">
+        <f>D2-B2</f>
         <v>28</v>
       </c>
-      <c r="C2" s="7">
+      <c r="F2" s="7">
+        <f>E2*C2</f>
         <v>28</v>
       </c>
-      <c r="D2" s="7">
+      <c r="G2" s="7">
+        <f>F2/24</f>
         <v>1.1666666666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B3" s="9">
+        <v>114</v>
+      </c>
+      <c r="C3" s="9">
+        <v>8</v>
+      </c>
+      <c r="D3" s="9">
+        <v>114</v>
+      </c>
+      <c r="E3" s="7">
+        <f t="shared" ref="E3:E18" si="0">D3-B3</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <f t="shared" ref="F3:F18" si="1">E3*C3</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <f t="shared" ref="G3:G18" si="2">F3/24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="8">
+        <v>30</v>
+      </c>
+      <c r="C4" s="8">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8">
+        <v>200</v>
+      </c>
+      <c r="E4" s="7">
+        <f t="shared" si="0"/>
         <v>170</v>
       </c>
-      <c r="C4" s="7">
+      <c r="F4" s="7">
+        <f t="shared" si="1"/>
         <v>1360</v>
       </c>
-      <c r="D4" s="7">
+      <c r="G4" s="7">
+        <f t="shared" si="2"/>
         <v>56.666666666666664</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="9">
+        <v>10</v>
+      </c>
+      <c r="C5" s="9">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9">
+        <v>150</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="C5" s="7">
+      <c r="F5" s="7">
+        <f t="shared" si="1"/>
         <v>1120</v>
       </c>
-      <c r="D5" s="7">
+      <c r="G5" s="7">
+        <f t="shared" si="2"/>
         <v>46.666666666666664</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="8">
+        <v>120</v>
+      </c>
+      <c r="C6" s="8">
+        <v>8</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1600</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="0"/>
         <v>1480</v>
       </c>
-      <c r="C6" s="7">
+      <c r="F6" s="7">
+        <f t="shared" si="1"/>
         <v>11840</v>
       </c>
-      <c r="D6" s="7">
+      <c r="G6" s="7">
+        <f t="shared" si="2"/>
         <v>493.33333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="9">
+        <v>200</v>
+      </c>
+      <c r="C7" s="9">
+        <v>8</v>
+      </c>
+      <c r="D7" s="9">
+        <v>3000</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="0"/>
         <v>2800</v>
       </c>
-      <c r="C7" s="7">
+      <c r="F7" s="7">
+        <f t="shared" si="1"/>
         <v>22400</v>
       </c>
-      <c r="D7" s="7">
+      <c r="G7" s="7">
+        <f t="shared" si="2"/>
         <v>933.33333333333337</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="8">
+        <v>50</v>
+      </c>
+      <c r="C8" s="8">
+        <v>8</v>
+      </c>
+      <c r="D8" s="8">
+        <v>150</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="C8" s="7">
+      <c r="F8" s="7">
+        <f t="shared" si="1"/>
         <v>800</v>
       </c>
-      <c r="D8" s="7">
+      <c r="G8" s="7">
+        <f t="shared" si="2"/>
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="7">
-        <v>0</v>
-      </c>
-      <c r="C9" s="7">
-        <v>0</v>
-      </c>
-      <c r="D9" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="8">
+        <v>500</v>
+      </c>
+      <c r="C10" s="8">
+        <v>8</v>
+      </c>
+      <c r="D10" s="8">
+        <v>48000</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="0"/>
         <v>47500</v>
       </c>
-      <c r="C10" s="7">
+      <c r="F10" s="7">
+        <f t="shared" si="1"/>
         <v>380000</v>
       </c>
-      <c r="D10" s="7">
+      <c r="G10" s="7">
+        <f t="shared" si="2"/>
         <v>15833.333333333334</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="7">
-        <v>0</v>
-      </c>
-      <c r="C11" s="7">
-        <v>0</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="8">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8">
+        <v>4</v>
+      </c>
+      <c r="D12" s="8">
+        <v>10</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C12" s="7">
+      <c r="F12" s="7">
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="D12" s="7">
+      <c r="G12" s="7">
+        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="9">
+        <v>100</v>
+      </c>
+      <c r="C13" s="9">
+        <v>8</v>
+      </c>
+      <c r="D13" s="9">
+        <v>5000</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
         <v>4900</v>
       </c>
-      <c r="C13" s="7">
+      <c r="F13" s="7">
+        <f t="shared" si="1"/>
         <v>39200</v>
       </c>
-      <c r="D13" s="7">
+      <c r="G13" s="7">
+        <f t="shared" si="2"/>
         <v>1633.3333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="8">
+        <v>50</v>
+      </c>
+      <c r="C14" s="8">
+        <v>8</v>
+      </c>
+      <c r="D14" s="8">
+        <v>500</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="0"/>
         <v>450</v>
       </c>
-      <c r="C14" s="7">
+      <c r="F14" s="7">
+        <f t="shared" si="1"/>
         <v>3600</v>
       </c>
-      <c r="D14" s="7">
+      <c r="G14" s="7">
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="9">
+        <v>30</v>
+      </c>
+      <c r="C15" s="9">
+        <v>8</v>
+      </c>
+      <c r="D15" s="9">
+        <v>100</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="C15" s="7">
+      <c r="F15" s="7">
+        <f t="shared" si="1"/>
         <v>560</v>
       </c>
-      <c r="D15" s="7">
+      <c r="G15" s="7">
+        <f t="shared" si="2"/>
         <v>23.333333333333332</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="8">
+        <v>50</v>
+      </c>
+      <c r="C16" s="8">
+        <v>8</v>
+      </c>
+      <c r="D16" s="8">
+        <v>170</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="C16" s="7">
+      <c r="F16" s="7">
+        <f t="shared" si="1"/>
         <v>960</v>
       </c>
-      <c r="D16" s="7">
+      <c r="G16" s="7">
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="9">
+        <v>40</v>
+      </c>
+      <c r="C17" s="9">
+        <v>8</v>
+      </c>
+      <c r="D17" s="9">
+        <v>130</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="C17" s="7">
+      <c r="F17" s="7">
+        <f t="shared" si="1"/>
         <v>720</v>
       </c>
-      <c r="D17" s="7">
+      <c r="G17" s="7">
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="8">
+        <v>100</v>
+      </c>
+      <c r="C18" s="8">
+        <v>8</v>
+      </c>
+      <c r="D18" s="8">
+        <v>350</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="C18" s="7">
+      <c r="F18" s="7">
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
-      <c r="D18" s="7">
+      <c r="G18" s="7">
+        <f t="shared" si="2"/>
         <v>83.333333333333329</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1343,478 +1565,280 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G18"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="8">
-        <v>2</v>
-      </c>
-      <c r="C2" s="8">
-        <v>1</v>
-      </c>
-      <c r="D2" s="8">
+      <c r="B2" s="7">
+        <v>28</v>
+      </c>
+      <c r="C2" s="7">
+        <v>28</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1.1666666666666667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7">
+        <v>170</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1360</v>
+      </c>
+      <c r="D4" s="7">
+        <v>56.666666666666664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="7">
+        <v>140</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1120</v>
+      </c>
+      <c r="D5" s="7">
+        <v>46.666666666666664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1480</v>
+      </c>
+      <c r="C6" s="7">
+        <v>11840</v>
+      </c>
+      <c r="D6" s="7">
+        <v>493.33333333333331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7">
+        <v>2800</v>
+      </c>
+      <c r="C7" s="7">
+        <v>22400</v>
+      </c>
+      <c r="D7" s="7">
+        <v>933.33333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="7">
-        <f>D2-B2</f>
+      <c r="B8" s="7">
+        <v>100</v>
+      </c>
+      <c r="C8" s="7">
+        <v>800</v>
+      </c>
+      <c r="D8" s="7">
+        <v>33.333333333333336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="7">
+        <v>47500</v>
+      </c>
+      <c r="C10" s="7">
+        <v>380000</v>
+      </c>
+      <c r="D10" s="7">
+        <v>15833.333333333334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="7">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7">
+        <v>36</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="7">
-        <f>E2*C2</f>
-        <v>28</v>
-      </c>
-      <c r="G2" s="7">
-        <f>F2/24</f>
-        <v>1.1666666666666667</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="9">
-        <v>114</v>
-      </c>
-      <c r="C3" s="9">
-        <v>8</v>
-      </c>
-      <c r="D3" s="9">
-        <v>114</v>
-      </c>
-      <c r="E3" s="7">
-        <f t="shared" ref="E3:E18" si="0">D3-B3</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="7">
-        <f t="shared" ref="F3:F18" si="1">E3*C3</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="7">
-        <f t="shared" ref="G3:G18" si="2">F3/24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="8">
+      <c r="B13" s="7">
+        <v>4900</v>
+      </c>
+      <c r="C13" s="7">
+        <v>39200</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1633.3333333333333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="7">
+        <v>450</v>
+      </c>
+      <c r="C14" s="7">
+        <v>3600</v>
+      </c>
+      <c r="D14" s="7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="7">
+        <v>70</v>
+      </c>
+      <c r="C15" s="7">
+        <v>560</v>
+      </c>
+      <c r="D15" s="7">
+        <v>23.333333333333332</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="7">
+        <v>120</v>
+      </c>
+      <c r="C16" s="7">
+        <v>960</v>
+      </c>
+      <c r="D16" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="7">
+        <v>90</v>
+      </c>
+      <c r="C17" s="7">
+        <v>720</v>
+      </c>
+      <c r="D17" s="7">
         <v>30</v>
       </c>
-      <c r="C4" s="8">
-        <v>8</v>
-      </c>
-      <c r="D4" s="8">
-        <v>200</v>
-      </c>
-      <c r="E4" s="7">
-        <f t="shared" si="0"/>
-        <v>170</v>
-      </c>
-      <c r="F4" s="7">
-        <f t="shared" si="1"/>
-        <v>1360</v>
-      </c>
-      <c r="G4" s="7">
-        <f t="shared" si="2"/>
-        <v>56.666666666666664</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="9">
-        <v>10</v>
-      </c>
-      <c r="C5" s="9">
-        <v>8</v>
-      </c>
-      <c r="D5" s="9">
-        <v>150</v>
-      </c>
-      <c r="E5" s="7">
-        <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="F5" s="7">
-        <f t="shared" si="1"/>
-        <v>1120</v>
-      </c>
-      <c r="G5" s="7">
-        <f t="shared" si="2"/>
-        <v>46.666666666666664</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="8">
-        <v>120</v>
-      </c>
-      <c r="C6" s="8">
-        <v>8</v>
-      </c>
-      <c r="D6" s="8">
-        <v>1600</v>
-      </c>
-      <c r="E6" s="7">
-        <f t="shared" si="0"/>
-        <v>1480</v>
-      </c>
-      <c r="F6" s="7">
-        <f t="shared" si="1"/>
-        <v>11840</v>
-      </c>
-      <c r="G6" s="7">
-        <f t="shared" si="2"/>
-        <v>493.33333333333331</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="9">
-        <v>200</v>
-      </c>
-      <c r="C7" s="9">
-        <v>8</v>
-      </c>
-      <c r="D7" s="9">
-        <v>3000</v>
-      </c>
-      <c r="E7" s="7">
-        <f t="shared" si="0"/>
-        <v>2800</v>
-      </c>
-      <c r="F7" s="7">
-        <f t="shared" si="1"/>
-        <v>22400</v>
-      </c>
-      <c r="G7" s="7">
-        <f t="shared" si="2"/>
-        <v>933.33333333333337</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="8">
-        <v>50</v>
-      </c>
-      <c r="C8" s="8">
-        <v>8</v>
-      </c>
-      <c r="D8" s="8">
-        <v>150</v>
-      </c>
-      <c r="E8" s="7">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F8" s="7">
-        <f t="shared" si="1"/>
-        <v>800</v>
-      </c>
-      <c r="G8" s="7">
-        <f t="shared" si="2"/>
-        <v>33.333333333333336</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="8">
-        <v>500</v>
-      </c>
-      <c r="C10" s="8">
-        <v>8</v>
-      </c>
-      <c r="D10" s="8">
-        <v>48000</v>
-      </c>
-      <c r="E10" s="7">
-        <f t="shared" si="0"/>
-        <v>47500</v>
-      </c>
-      <c r="F10" s="7">
-        <f t="shared" si="1"/>
-        <v>380000</v>
-      </c>
-      <c r="G10" s="7">
-        <f t="shared" si="2"/>
-        <v>15833.333333333334</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="9">
-        <v>1</v>
-      </c>
-      <c r="C11" s="9">
-        <v>1</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1</v>
-      </c>
-      <c r="E11" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="8">
-        <v>1</v>
-      </c>
-      <c r="C12" s="8">
-        <v>4</v>
-      </c>
-      <c r="D12" s="8">
-        <v>10</v>
-      </c>
-      <c r="E12" s="7">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="F12" s="7">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="G12" s="7">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="9">
-        <v>100</v>
-      </c>
-      <c r="C13" s="9">
-        <v>8</v>
-      </c>
-      <c r="D13" s="9">
-        <v>5000</v>
-      </c>
-      <c r="E13" s="7">
-        <f t="shared" si="0"/>
-        <v>4900</v>
-      </c>
-      <c r="F13" s="7">
-        <f t="shared" si="1"/>
-        <v>39200</v>
-      </c>
-      <c r="G13" s="7">
-        <f t="shared" si="2"/>
-        <v>1633.3333333333333</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="8">
-        <v>50</v>
-      </c>
-      <c r="C14" s="8">
-        <v>8</v>
-      </c>
-      <c r="D14" s="8">
-        <v>500</v>
-      </c>
-      <c r="E14" s="7">
-        <f t="shared" si="0"/>
-        <v>450</v>
-      </c>
-      <c r="F14" s="7">
-        <f t="shared" si="1"/>
-        <v>3600</v>
-      </c>
-      <c r="G14" s="7">
-        <f t="shared" si="2"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="9">
-        <v>30</v>
-      </c>
-      <c r="C15" s="9">
-        <v>8</v>
-      </c>
-      <c r="D15" s="9">
-        <v>100</v>
-      </c>
-      <c r="E15" s="7">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="F15" s="7">
-        <f t="shared" si="1"/>
-        <v>560</v>
-      </c>
-      <c r="G15" s="7">
-        <f t="shared" si="2"/>
-        <v>23.333333333333332</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="8">
-        <v>50</v>
-      </c>
-      <c r="C16" s="8">
-        <v>8</v>
-      </c>
-      <c r="D16" s="8">
-        <v>170</v>
-      </c>
-      <c r="E16" s="7">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="F16" s="7">
-        <f t="shared" si="1"/>
-        <v>960</v>
-      </c>
-      <c r="G16" s="7">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="9">
-        <v>40</v>
-      </c>
-      <c r="C17" s="9">
-        <v>8</v>
-      </c>
-      <c r="D17" s="9">
-        <v>130</v>
-      </c>
-      <c r="E17" s="7">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="F17" s="7">
-        <f t="shared" si="1"/>
-        <v>720</v>
-      </c>
-      <c r="G17" s="7">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="8">
-        <v>100</v>
-      </c>
-      <c r="C18" s="8">
-        <v>8</v>
-      </c>
-      <c r="D18" s="8">
-        <v>350</v>
-      </c>
-      <c r="E18" s="7">
-        <f t="shared" si="0"/>
+      <c r="B18" s="7">
         <v>250</v>
       </c>
-      <c r="F18" s="7">
-        <f t="shared" si="1"/>
+      <c r="C18" s="7">
         <v>2000</v>
       </c>
-      <c r="G18" s="7">
-        <f t="shared" si="2"/>
+      <c r="D18" s="7">
         <v>83.333333333333329</v>
       </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2273,4 +2297,718 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R4" sqref="A1:R4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="8">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9">
+        <v>114</v>
+      </c>
+      <c r="D2" s="8">
+        <v>30</v>
+      </c>
+      <c r="E2" s="9">
+        <v>10</v>
+      </c>
+      <c r="F2" s="8">
+        <v>120</v>
+      </c>
+      <c r="G2" s="9">
+        <v>200</v>
+      </c>
+      <c r="H2" s="8">
+        <v>50</v>
+      </c>
+      <c r="I2" s="9">
+        <v>1</v>
+      </c>
+      <c r="J2" s="8">
+        <v>500</v>
+      </c>
+      <c r="K2" s="9">
+        <v>1</v>
+      </c>
+      <c r="L2" s="8">
+        <v>1</v>
+      </c>
+      <c r="M2" s="9">
+        <v>100</v>
+      </c>
+      <c r="N2" s="8">
+        <v>50</v>
+      </c>
+      <c r="O2" s="9">
+        <v>30</v>
+      </c>
+      <c r="P2" s="8">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>40</v>
+      </c>
+      <c r="R2" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="8">
+        <v>30</v>
+      </c>
+      <c r="C3" s="9">
+        <v>114</v>
+      </c>
+      <c r="D3" s="8">
+        <v>200</v>
+      </c>
+      <c r="E3" s="9">
+        <v>150</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1600</v>
+      </c>
+      <c r="G3" s="9">
+        <v>3000</v>
+      </c>
+      <c r="H3" s="8">
+        <v>150</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1</v>
+      </c>
+      <c r="J3" s="8">
+        <v>48000</v>
+      </c>
+      <c r="K3" s="9">
+        <v>1</v>
+      </c>
+      <c r="L3" s="8">
+        <v>10</v>
+      </c>
+      <c r="M3" s="9">
+        <v>5000</v>
+      </c>
+      <c r="N3" s="8">
+        <v>500</v>
+      </c>
+      <c r="O3" s="9">
+        <v>100</v>
+      </c>
+      <c r="P3" s="8">
+        <v>170</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>130</v>
+      </c>
+      <c r="R3" s="8">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="7">
+        <f>B3-B2</f>
+        <v>28</v>
+      </c>
+      <c r="C4" s="7">
+        <f>C3-C2</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <f>D3-D2</f>
+        <v>170</v>
+      </c>
+      <c r="E4" s="7">
+        <f>E3-E2</f>
+        <v>140</v>
+      </c>
+      <c r="F4" s="7">
+        <f>F3-F2</f>
+        <v>1480</v>
+      </c>
+      <c r="G4" s="7">
+        <f>G3-G2</f>
+        <v>2800</v>
+      </c>
+      <c r="H4" s="7">
+        <f>H3-H2</f>
+        <v>100</v>
+      </c>
+      <c r="I4" s="7">
+        <f>I3-I2</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <f>J3-J2</f>
+        <v>47500</v>
+      </c>
+      <c r="K4" s="7">
+        <f>K3-K2</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <f>L3-L2</f>
+        <v>9</v>
+      </c>
+      <c r="M4" s="7">
+        <f>M3-M2</f>
+        <v>4900</v>
+      </c>
+      <c r="N4" s="7">
+        <f>N3-N2</f>
+        <v>450</v>
+      </c>
+      <c r="O4" s="7">
+        <f>O3-O2</f>
+        <v>70</v>
+      </c>
+      <c r="P4" s="7">
+        <f>P3-P2</f>
+        <v>120</v>
+      </c>
+      <c r="Q4" s="7">
+        <f>Q3-Q2</f>
+        <v>90</v>
+      </c>
+      <c r="R4" s="7">
+        <f>R3-R2</f>
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="8">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="9">
+        <v>114</v>
+      </c>
+      <c r="C3" s="9">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="8">
+        <v>30</v>
+      </c>
+      <c r="C4" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="9">
+        <v>10</v>
+      </c>
+      <c r="C5" s="9">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="8">
+        <v>120</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="9">
+        <v>200</v>
+      </c>
+      <c r="C7" s="9">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="8">
+        <v>50</v>
+      </c>
+      <c r="C8" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="8">
+        <v>500</v>
+      </c>
+      <c r="C10" s="8">
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="9">
+        <v>100</v>
+      </c>
+      <c r="C13" s="9">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="8">
+        <v>50</v>
+      </c>
+      <c r="C14" s="8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="9">
+        <v>30</v>
+      </c>
+      <c r="C15" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="8">
+        <v>50</v>
+      </c>
+      <c r="C16" s="8">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="9">
+        <v>40</v>
+      </c>
+      <c r="C17" s="9">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="8">
+        <v>100</v>
+      </c>
+      <c r="C18" s="8">
+        <v>350</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9">
+        <v>8</v>
+      </c>
+      <c r="D2" s="8">
+        <v>8</v>
+      </c>
+      <c r="E2" s="9">
+        <v>8</v>
+      </c>
+      <c r="F2" s="8">
+        <v>8</v>
+      </c>
+      <c r="G2" s="9">
+        <v>8</v>
+      </c>
+      <c r="H2" s="8">
+        <v>8</v>
+      </c>
+      <c r="I2" s="9">
+        <v>1</v>
+      </c>
+      <c r="J2" s="8">
+        <v>8</v>
+      </c>
+      <c r="K2" s="9">
+        <v>1</v>
+      </c>
+      <c r="L2" s="8">
+        <v>4</v>
+      </c>
+      <c r="M2" s="9">
+        <v>8</v>
+      </c>
+      <c r="N2" s="8">
+        <v>8</v>
+      </c>
+      <c r="O2" s="9">
+        <v>8</v>
+      </c>
+      <c r="P2" s="8">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>8</v>
+      </c>
+      <c r="R2" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="7">
+        <v>28</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1360</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1120</v>
+      </c>
+      <c r="F3" s="7">
+        <v>11840</v>
+      </c>
+      <c r="G3" s="7">
+        <v>22400</v>
+      </c>
+      <c r="H3" s="7">
+        <v>800</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
+        <v>380000</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7">
+        <v>36</v>
+      </c>
+      <c r="M3" s="7">
+        <v>39200</v>
+      </c>
+      <c r="N3" s="7">
+        <v>3600</v>
+      </c>
+      <c r="O3" s="7">
+        <v>560</v>
+      </c>
+      <c r="P3" s="7">
+        <v>960</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>720</v>
+      </c>
+      <c r="R3" s="7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>56.666666666666664</v>
+      </c>
+      <c r="E4" s="7">
+        <v>46.666666666666664</v>
+      </c>
+      <c r="F4" s="7">
+        <v>493.33333333333331</v>
+      </c>
+      <c r="G4" s="7">
+        <v>933.33333333333337</v>
+      </c>
+      <c r="H4" s="7">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <v>15833.333333333334</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="M4" s="7">
+        <v>1633.3333333333333</v>
+      </c>
+      <c r="N4" s="7">
+        <v>150</v>
+      </c>
+      <c r="O4" s="7">
+        <v>23.333333333333332</v>
+      </c>
+      <c r="P4" s="7">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>30</v>
+      </c>
+      <c r="R4" s="7">
+        <v>83.333333333333329</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>